<commit_message>
sample input data change
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\excel-product-cleaner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C48DD42-88B8-4536-81CF-6A0B3723AAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A16523D-4E56-4CDB-9E53-A74B190817B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29925" yWindow="-600" windowWidth="21600" windowHeight="12645" xr2:uid="{F1225FE0-BA30-41CD-83D4-928214C21203}"/>
   </bookViews>
@@ -36,7 +36,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>additional_attributes</t>
+  </si>
   <si>
     <t>color=Black,mb_hover_img=/x/i/xiaomi_12_lite_back_1.png,specifications=Ram&lt;br /&gt;Rom&lt;br /&gt;Battery&lt;br /&gt;Disply Camera</t>
   </si>
@@ -91,38 +94,6 @@
 &lt;p&gt;Â &lt;/p&gt;_x000D_
 &lt;p&gt;Â &lt;/p&gt;_x000D_
 &lt;p&gt;Â &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>color=Gray,mb_hover_img=/g/r/gray_1__1_1.png,specifications=&lt;p&gt;Model: Tab 70 WiFi&lt;br /&gt;Color:Â  Â Space Grey, Twilight Blue&lt;br /&gt;Dimension:Â  Â 246.5*163*9.9mm&lt;br /&gt;Weight:Â  Â 520.5g&lt;br /&gt;Display:Â  Â 10.1-inch 800*1280 HD+ IPS 79% Screen-to-body Ratio&lt;br /&gt;CPU:Â  Â  Quad-core Rockchip RK3562&lt;br /&gt;RAM &amp; ROM:Â  Â  3GB+64GB, LPDDR3 + EMMC5.1 Up to 3GB RAM Expansion&lt;br /&gt;Max TF Card Capacity:Â  Â  1TB&lt;br /&gt;OS:Â  Â  DokeOS_P 3.0 Based on Android 13&lt;br /&gt;Rear Camera:Â  Â  5MP&lt;br /&gt;Front Camera:Â  Â  2MP&lt;br /&gt;Battery Capacity:Â  Â  6580mAh&lt;br /&gt;Speaker:Â  Â  1217 2PCS BOX Speakers&lt;br /&gt;Wi-Fi:Â  Â  802.11a/b/g/n/ac/ax&lt;br /&gt;Bluetooth version:Â  Â  BT5.0&lt;br /&gt;&lt;br /&gt;&lt;/p&gt;_x000D_
-&lt;p&gt;Â &lt;/p&gt;_x000D_
-&lt;p&gt;Â &lt;/p&gt;_x000D_
-&lt;p&gt;Â &lt;/p&gt;_x000D_
-&lt;p&gt;Â &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>color=Blue,mb_hover_img=/w/h/whatsapp_image_2024-04-17_at_15.24.04_1d58a050.jpg,specifications=&lt;p&gt;Model: Tab 70 WiFi&lt;br /&gt;Color:Â  Â Space Grey, Twilight Blue&lt;br /&gt;Dimension:Â  Â 246.5*163*9.9mm&lt;br /&gt;Weight:Â  Â 520.5g&lt;br /&gt;Display:Â  Â 10.1-inch 800*1280 HD+ IPS 79% Screen-to-body Ratio&lt;br /&gt;CPU:Â  Â  Quad-core Rockchip RK3562&lt;br /&gt;RAM &amp; ROM:Â  Â  3GB+64GB, LPDDR3 + EMMC5.1 Up to 3GB RAM Expansion&lt;br /&gt;Max TF Card Capacity:Â  Â  1TB&lt;br /&gt;OS:Â  Â  DokeOS_P 3.0 Based on Android 13&lt;br /&gt;Rear Camera:Â  Â  5MP&lt;br /&gt;Front Camera:Â  Â  2MP&lt;br /&gt;Battery Capacity:Â  Â  6580mAh&lt;br /&gt;Speaker:Â  Â  1217 2PCS BOX Speakers&lt;br /&gt;Wi-Fi:Â  Â  802.11a/b/g/n/ac/ax&lt;br /&gt;Bluetooth version:Â  Â  BT5.0&lt;br /&gt;&lt;br /&gt;&lt;/p&gt;_x000D_
-&lt;p&gt;Â &lt;/p&gt;_x000D_
-&lt;p&gt;Â &lt;/p&gt;_x000D_
-&lt;p&gt;Â &lt;/p&gt;_x000D_
-&lt;p&gt;Â &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>mb_hover_img=/b/l/blue_3__1_2.png</t>
-  </si>
-  <si>
-    <t>mb_hover_img=/1/_/1_10.png,ram=8GB,rom=256GB,processor=&lt;span&gt;The POCO C65 is powered by the MediaTek Helio G85 processor, designed for a balance between performance and power efficiency, suitable for gaming and daily useâ€‹&lt;/span&gt;&lt;span class="" data-state="closed"&gt;&lt;a href="https://www.mi.com/uk/product/poco-c65/" target="_blank" rel="noopener noreferrer" class="text-green-600 !no-underline px-0.5"&gt;&lt;/a&gt;&lt;/span&gt;&lt;span&gt;â€‹.&lt;/span&gt;,rear_camera=&lt;span&gt;The POCO C65 is equipped with a 50MP AI triple camera setup, designed to capture high-quality photos with enhanced details and clarityâ€‹&lt;/span&gt;&lt;span class="" data-state="closed"&gt;&lt;a href="https://www.mi.com/uk/product/poco-c65/" target="_blank" rel="noopener noreferrer" class="text-green-600 !no-underline px-0.5"&gt;&lt;/a&gt;&lt;/span&gt;&lt;span&gt;â€‹.&lt;/span&gt;,front_camera=&lt;span data-key="spec_44" class="xm-text f-bold " data-type="text" data-id="4ad32f1282"&gt;Film Filter &lt;br /&gt;Â HDR mode&lt;br /&gt;Â Soft-light ring &lt;br /&gt;Â Portrait mode &lt;br /&gt;Â Time-lapse&lt;/span&gt;&lt;span data-key="spec_45" class="xm-text f-bold " data-type="text" data-id="985bdaa1cc"&gt;8MP front camera&lt;/span&gt;&lt;span data-key="spec_46" class="xm-text f-light " data-type="text" data-id="50239945c8"&gt;f/2.0&lt;/span&gt;,display=&lt;span&gt;The display on the POCO C65 is a 6.74" screen with a 90Hz refresh rate, designed for smooth scrolling and enhanced visual experience&lt;/span&gt;,battery_charging=&lt;span&gt;Â is equipped with a large 5000mAh battery, designed to support prolonged usage. It also supports 18W fast charging, enabling quick power-ups to keep you connected and productive throughout the day. This combination offers a balance between durability and convenience, making it suitable for extensive daily use.&lt;/span&gt;,cooling_system=The POCO C65's specific cooling system details are not mentioned in the available information. For cooling features or technologies used to manage heat during intensive operations,security_authentication=&lt;span&gt;For the POCO C65, security and authentication features typically include options like fingerprint sensors, face unlock, and possibly in-built software security measures to protect user data. These features ensure secure access to the device and safeguard personal information&lt;/span&gt;,nfc=supports multifunctional NFC, enabling convenient features like contactless payments, quick pairing with compatible devices, and easy data sharing.,network_connectivity=&lt;span&gt;The POCO C65 includes various network and connectivity options like 4G LTE, Wi-Fi, Bluetooth, and GPS. It also features multifunctional NFC for contactless transactions and device pairing&lt;/span&gt;,navigation=&lt;span&gt;The POCO C65 supports GPS, A-GPS, GLONASS, Beidou, and Galileo for comprehensive and accurate navigation capabilities, ensuring reliable location tracking across different regions and conditions&lt;/span&gt;,audio=&lt;span&gt;The POCO C65 features an audio system designed to deliver clear and immersive sound quality. It includes a 3.5mm headphone jack for compatibility with traditional wired headphones, ensuring users have flexibility in their choice of audio output.&lt;/span&gt;,sensor=&lt;strong&gt;&lt;span&gt;Virtual proximity sensor | Ambient light sensor | Accelerometer | Electronic compass&lt;/span&gt;&lt;/strong&gt;,operating_system=MIUI 14 for POCO*Availability of MIUI features, apps and services may vary depending on software version and phone model.,package_contents=Mobile Phone / Adapter / USB Type-C Cable / SIM Eject Tool / Quick Start Guide and Warranty Card / Safety Information*Contents in the package may differ across different regions.,rear_video_recording=&lt;span&gt;The POCO C65 supports front video recording, enhancing your video capturing capabilities.&lt;/span&gt;,video_playback=&lt;span&gt;The POCO C65 supports video playback, offering a great visual experience with its 6.74" HD+ display and 90Hz refresh rate.&lt;/span&gt;,data_transfer=&lt;span&gt;The POCO C65 offers data transfer features such as multifunctional NFC, a Type-C port for modern connectivity, and a 3.5mm headphone jack for traditional audio devices. These features facilitate versatile data sharing and connectivity options for users&lt;/span&gt;,dimensions=&lt;span data-key="spec_17" class="xm-text f-light " data-type="text" data-id="e30aa33e0b"&gt;Height: 168mm &lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_18" class="xm-text f-light " data-type="text" data-id="4324f2c478"&gt;Width: 78mm&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_19" class="xm-text f-light " data-type="text" data-id="c9750e593e"&gt;Thickness: 8.09mm&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_20" class="xm-text f-light " data-type="text" data-id="fdc5d72901"&gt;Weight: 192g&lt;/span&gt;&lt;span data-key="spec_21" class="xm-text f-light " data-type="text" data-id="bed668186a"&gt;*&lt;br /&gt;Data obtained from POCO laboratory. Industry measurement methods may vary, and therefore actual results may differ.&lt;/span&gt;,specifications=&lt;span&gt;The POCO C65 features a MediaTek Helio G85 processor, 6.74" 90Hz display, 50MP AI triple camera, 5000mAh battery, 18W fast charging, up to 16GB RAM with memory extension, 1TB storage expansion, side fingerprint sensor, and runs on MIUI 14 for POCOâ€‹&lt;/span&gt;&lt;span class="" data-state="closed"&gt;&lt;a href="https://www.mi.com/uk/product/poco-c65/" target="_blank" rel="noopener noreferrer" class="text-green-600 !no-underline px-0.5"&gt;&lt;/a&gt;&lt;/span&gt;&lt;span&gt;â€‹.&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>mb_hover_img=/1/_/1_10_2.png,ram=12GB,rom=512GB,processor=&lt;span data-key="spec_5" class="xm-text f-bold " data-type="text" data-id="effc52d893"&gt;Helio G99-Ultra&lt;/span&gt;&lt;span data-key="spec_6" class="xm-text f-light " data-type="text" data-id="0e3223a7ee"&gt;TSMC 6nm manufacturing process&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_7" class="xm-text f-light " data-type="text" data-id="308b50a033"&gt;CPUï¼š Octa-core processor 2 x Arm Cortex-A76, up to 2.2GHz 6 x Arm Cortex-A55, up to 2.0GHz&lt;/span&gt;&lt;span data-key="spec_8" class="xm-text f-light " data-type="text" data-id="a5c9ae0379"&gt;GPUï¼š ARM Mali-G57 MC2&lt;/span&gt;,rear_camera=&lt;span&gt;64MP+8MP+2MP triple camera&amp;nbsp;&lt;br&gt;&lt;span data-key="spec_46" class="xm-text f-bold " data-type="text" data-id="e800562df3"&gt;Rear camera photography features&lt;/span&gt;&lt;span data-key="spec_47" class="xm-text f-light " data-type="text" data-id="9c3b31007e"&gt;64MP mode | Night mode | Document mode | Film Camera | Portrait mode&lt;/span&gt;&lt;br&gt;&lt;/span&gt;,front_camera=&lt;span data-key="spec_57" class="xm-text f-bold " data-type="text" data-id="4ad32f1282"&gt;16MP front camera&lt;/span&gt;&lt;span data-key="spec_58" class="xm-text f-light " data-type="text" data-id="985bdaa1cc"&gt;f/2.45&amp;nbsp;&lt;br&gt;&lt;span data-key="spec_59" class="xm-text f-bold " data-type="text" data-id="2fdf4269c7"&gt;Front camera photography features &lt;br&gt;&lt;/span&gt;Night mode&lt;br&gt;Film Camera&lt;br&gt;Portrait mode&lt;br&gt;&lt;/span&gt;,display=&lt;span data-key="spec_22" class="xm-text f-bold " data-type="text" data-id="62023a1c0e"&gt;6.67" FHD+ Flow AMOLED DotDisplay&lt;/span&gt;&lt;span data-key="spec_23" class="xm-text f-light " data-type="text" data-id="6325f86c00"&gt;2400*1080, 394 ppi&lt;/span&gt;&lt;span data-key="spec_24" class="xm-text f-light " data-type="text" data-id="09007bdcc5"&gt;Contrast ratio: 5,000,000:1&lt;/span&gt;&lt;span data-key="spec_25" class="xm-text f-light " data-type="text" data-id="f031d76f85"&gt;Colour gamut: DCI-P3 wide colour gamut&lt;/span&gt;&lt;span data-key="spec_26" class="xm-text f-light " data-type="text" data-id="02324a2365"&gt;Brightness: 1000 nits (HBM), 1300 nits (peak)&lt;/span&gt;&lt;span data-key="spec_27" class="xm-text f-light " data-type="text" data-id="39feed82bf"&gt;Refresh rate: Up to 120Hz&lt;/span&gt;,battery_charging=&lt;span data-key="spec_70" class="xm-text f-light " data-type="text" data-id="4535c816f1"&gt;5000mAh (typ)&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_71" class="xm-text f-light " data-type="text" data-id="e2705627e0"&gt;67W wired turbo charging&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_72" class="xm-text f-light " data-type="text" data-id="264439ae59"&gt;67W in-box charger &lt;/span&gt;&lt;span data-key="spec_73" class="xm-text f-light " data-type="text" data-id="3b4b27fa9e"&gt;USB-C&lt;/span&gt;,cooling_system=The POCO M6 Pro features an advanced cooling system designed for optimal heat dissipation, ensuring smooth performance and preventing overheating during intensive use,security_authentication=&lt;span data-key="spec_75" class="xm-text f-light " data-type="text" data-id="0dc0744ecd"&gt;&lt;span&gt;The POCO M6 Pro includes security and authentication features to protect user data and ensure privacy&lt;/span&gt;&lt;br&gt;&lt;br&gt;In-screen fingerprint sensor&lt;br&gt;&lt;/span&gt;&lt;span data-key="spec_76" class="xm-text f-light " data-type="text" data-id="8cae001ad8"&gt;AI Face Unlock&lt;/span&gt;,nfc= enabling wireless communication between devices over short distances. This feature facilitates contactless payments, easy pairing with compatible devices, and quick data sharing.,network_connectivity=&lt;span&gt;&lt;br&gt;SIM1 + Hybrid* (SIM or MicroSD), supports dual 4G&lt;br&gt;&amp;nbsp;offers comprehensive network and connectivity options, ensuring users can stay connected in various environments and with multiple devices. It supports dual SIM functionality, allowing for versatile network usage.&lt;/span&gt;,navigation=&lt;span&gt;&lt;br&gt;GPS: L1 ï½œGLONASS: G1 | BDS: B1 | Galileo: E1&lt;br&gt;includes navigation features that utilize various satellite systems for accurate location tracking and mapping.&lt;/span&gt;,audio=&lt;span data-key="spec_95" class="xm-text f-light " data-type="text" data-id="544669ec9d"&gt;Dual speakers&lt;/span&gt;&lt;span data-key="spec_96" class="xm-text f-light " data-type="text" data-id="565928f0d8"&gt;3.5mm&amp;nbsp;&lt;br&gt;headphone jack&lt;br&gt;&lt;/span&gt;&lt;span data-key="spec_97" class="xm-text f-light " data-type="text" data-id="a78985a8a9"&gt;Dolby Atmos certification&lt;br&gt;&lt;/span&gt;&lt;span data-key="spec_98" class="xm-text f-light " data-type="text" data-id="5ba3fc8546"&gt;Hi-Res Audio certification&lt;br&gt;&lt;/span&gt;&lt;span data-key="spec_99" class="xm-text f-light " data-type="text" data-id="6ec848d980"&gt;Supports audio formats such as MP3 | FLAC | AAC | OGG | WAV&lt;/span&gt;,splash_water_dust_resistance=&lt;span data-key="spec_103" class="xm-text f-light " data-type="text" data-id="b39e83fc5b"&gt;IP54&lt;/span&gt;&lt;span data-key="spec_104" class="xm-text f-light " data-type="text" data-id="85040080f7"&gt;* &lt;br&gt;The device has been tested in a controlled environment and certified to be resistant to splash and dust in specific laboratory conditions with the classification IP54 under IEC 60529: 1989+A1:1999+A2:2013. Resistance is not permanent and may deteriorate naturally over time. If your device is wet, do not attempt to charge it. The life scene is different from the experimental environment. Do not immerse your smartphone in water completely or expose it to solutions such as seawater and chlorinated water or liquids such as drinks during daily use. Your warranty does not cover the damage caused by man-made immersion of your device in liquid. The test is conducted by TÃœV SÃœD Certification and Testing (China) Co., Ltd. Jiangsu Branch.&lt;/span&gt;,sensor=&lt;span&gt;The POCO M6 Pro is equipped with various sensors to enhance user experience and device functionality.&lt;br&gt;&lt;br&gt;Proximity sensor | Ambient light sensor | Accelerometer | Electronic compass | IR blaster ï½œGyroscope | Z-axis linear vibration motor&lt;/span&gt;,operating_system=MIUI 14 for POCO,rear_video_recording=&lt;span data-key="spec_52" class="xm-text f-bold " data-type="text" data-id="66c1cb5555"&gt;Rear camera video recording&lt;/span&gt;&lt;span data-key="spec_53" class="xm-text f-light " data-type="text" data-id="d36b6def57"&gt;1080p 1920Ã—1080 at 30fps/60fps&lt;/span&gt;&lt;span data-key="spec_54" class="xm-text f-light " data-type="text" data-id="314031b7bf"&gt;720p 1280Ã—720 at 30fps&lt;/span&gt;&lt;span data-key="spec_55" class="xm-text f-light " data-type="text" data-id="ff5535ab27"&gt;Slow motion video: 120fps, 720p&lt;/span&gt;,front_video_recording=&lt;span data-key="spec_66" class="xm-text f-bold " data-type="text" data-id="b07e125ed7"&gt;Front camera video recording&lt;/span&gt;&lt;span data-key="spec_67" class="xm-text f-light " data-type="text" data-id="4382a12439"&gt;1080p 1920Ã—1080 at 30fps/60fps&lt;/span&gt;&lt;span data-key="spec_68" class="xm-text f-light " data-type="text" data-id="c3aec946ef"&gt;720p 1280Ã—720 at 30fps&lt;/span&gt;,video_playback=&lt;span&gt;The POCO M6 Pro offers video playback capabilities designed to provide a high-quality viewing experience.&lt;/span&gt;,audio_playback=&lt;span&gt;The POCO M6 Pro is designed to provide an excellent audio playback experience.&lt;/span&gt;,data_transfer=&lt;span&gt;The POCO M6 Pro supports high-speed data transfer, ensuring swift and efficient file movement. This capability enhances user experience by reducing the time needed for data sharing between the device and other platforms or devices.&lt;/span&gt;,dimensions=&lt;span data-key="spec_16" class="xm-text f-light " data-type="text" data-id="e30aa33e0b"&gt;Height: 161.1mm&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_17" class="xm-text f-light " data-type="text" data-id="4324f2c478"&gt;Width: 74.95mm&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_18" class="xm-text f-light " data-type="text" data-id="c9750e593e"&gt;Thickness: 7.98mm&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_19" class="xm-text f-light " data-type="text" data-id="fdc5d72901"&gt;Weight: 179g&lt;/span&gt;,specifications=&lt;span&gt;The POCO M6 Pro specs include a high-performance Helio G99 processor, ample storage and memory options, a large and vibrant AMOLED display, high-resolution cameras, and fast charging capabilities, alongside features like NFC, dual SIM support, and splash resistance, all powered by a user-friendly MIUI interface.&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>color=Black,ram=8GB,rom=256GB,processor=&lt;span&gt;The POCO C65 is powered by the MediaTek Helio G85 processor, designed for a balance between performance and power efficiency, suitable for gaming and daily useâ€‹&lt;/span&gt;&lt;span class="" data-state="closed"&gt;&lt;a href="https://www.mi.com/uk/product/poco-c65/" target="_blank" rel="noopener noreferrer" class="text-green-600 !no-underline px-0.5"&gt;&lt;/a&gt;&lt;/span&gt;&lt;span&gt;â€‹.&lt;/span&gt;,rear_camera=&lt;span&gt;The POCO C65 is equipped with a 50MP AI triple camera setup, designed to capture high-quality photos with enhanced details and clarityâ€‹&lt;/span&gt;&lt;span class="" data-state="closed"&gt;&lt;a href="https://www.mi.com/uk/product/poco-c65/" target="_blank" rel="noopener noreferrer" class="text-green-600 !no-underline px-0.5"&gt;&lt;/a&gt;&lt;/span&gt;&lt;span&gt;â€‹.&lt;/span&gt;,front_camera=&lt;span data-key="spec_44" class="xm-text f-bold " data-type="text" data-id="4ad32f1282"&gt;Film Filter &lt;br /&gt;Â HDR mode&lt;br /&gt;Â Soft-light ring &lt;br /&gt;Â Portrait mode &lt;br /&gt;Â Time-lapse&lt;/span&gt;&lt;span data-key="spec_45" class="xm-text f-bold " data-type="text" data-id="985bdaa1cc"&gt;8MP front camera&lt;/span&gt;&lt;span data-key="spec_46" class="xm-text f-light " data-type="text" data-id="50239945c8"&gt;f/2.0&lt;/span&gt;,display=&lt;span&gt;The display on the POCO C65 is a 6.74" screen with a 90Hz refresh rate, designed for smooth scrolling and enhanced visual experience&lt;/span&gt;,battery_charging=&lt;span&gt;Â is equipped with a large 5000mAh battery, designed to support prolonged usage. It also supports 18W fast charging, enabling quick power-ups to keep you connected and productive throughout the day. This combination offers a balance between durability and convenience, making it suitable for extensive daily use.&lt;/span&gt;,cooling_system=The POCO C65's specific cooling system details are not mentioned in the available information. For cooling features or technologies used to manage heat during intensive operations,security_authentication=&lt;span&gt;For the POCO C65, security and authentication features typically include options like fingerprint sensors, face unlock, and possibly in-built software security measures to protect user data. These features ensure secure access to the device and safeguard personal information&lt;/span&gt;,nfc=supports multifunctional NFC, enabling convenient features like contactless payments, quick pairing with compatible devices, and easy data sharing.,network_connectivity=&lt;span&gt;The POCO C65 includes various network and connectivity options like 4G LTE, Wi-Fi, Bluetooth, and GPS. It also features multifunctional NFC for contactless transactions and device pairing&lt;/span&gt;,navigation=&lt;span&gt;The POCO C65 supports GPS, A-GPS, GLONASS, Beidou, and Galileo for comprehensive and accurate navigation capabilities, ensuring reliable location tracking across different regions and conditions&lt;/span&gt;,audio=&lt;span&gt;The POCO C65 features an audio system designed to deliver clear and immersive sound quality. It includes a 3.5mm headphone jack for compatibility with traditional wired headphones, ensuring users have flexibility in their choice of audio output.&lt;/span&gt;,sensor=&lt;strong&gt;&lt;span&gt;Virtual proximity sensor | Ambient light sensor | Accelerometer | Electronic compass&lt;/span&gt;&lt;/strong&gt;,operating_system=MIUI 14 for POCO*Availability of MIUI features, apps and services may vary depending on software version and phone model.,package_contents=Mobile Phone / Adapter / USB Type-C Cable / SIM Eject Tool / Quick Start Guide and Warranty Card / Safety Information*Contents in the package may differ across different regions.,rear_video_recording=&lt;span&gt;The POCO C65 supports front video recording, enhancing your video capturing capabilities.&lt;/span&gt;,video_playback=&lt;span&gt;The POCO C65 supports video playback, offering a great visual experience with its 6.74" HD+ display and 90Hz refresh rate.&lt;/span&gt;,data_transfer=&lt;span&gt;The POCO C65 offers data transfer features such as multifunctional NFC, a Type-C port for modern connectivity, and a 3.5mm headphone jack for traditional audio devices. These features facilitate versatile data sharing and connectivity options for users&lt;/span&gt;,dimensions=&lt;span data-key="spec_17" class="xm-text f-light " data-type="text" data-id="e30aa33e0b"&gt;Height: 168mm &lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_18" class="xm-text f-light " data-type="text" data-id="4324f2c478"&gt;Width: 78mm&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_19" class="xm-text f-light " data-type="text" data-id="c9750e593e"&gt;Thickness: 8.09mm&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_20" class="xm-text f-light " data-type="text" data-id="fdc5d72901"&gt;Weight: 192g&lt;/span&gt;&lt;span data-key="spec_21" class="xm-text f-light " data-type="text" data-id="bed668186a"&gt;*&lt;br /&gt;Data obtained from POCO laboratory. Industry measurement methods may vary, and therefore actual results may differ.&lt;/span&gt;,specifications=&lt;span&gt;The POCO C65 features a MediaTek Helio G85 processor, 6.74" 90Hz display, 50MP AI triple camera, 5000mAh battery, 18W fast charging, up to 16GB RAM with memory extension, 1TB storage expansion, side fingerprint sensor, and runs on MIUI 14 for POCOâ€‹&lt;/span&gt;&lt;span class="" data-state="closed"&gt;&lt;a href="https://www.mi.com/uk/product/poco-c65/" target="_blank" rel="noopener noreferrer" class="text-green-600 !no-underline px-0.5"&gt;&lt;/a&gt;&lt;/span&gt;&lt;span&gt;â€‹.&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>color=Purple,ram=8GB,rom=256GB,processor=&lt;span&gt;The POCO C65 is powered by the MediaTek Helio G85 processor, designed for a balance between performance and power efficiency, suitable for gaming and daily useâ€‹&lt;/span&gt;&lt;span class="" data-state="closed"&gt;&lt;a href="https://www.mi.com/uk/product/poco-c65/" target="_blank" rel="noopener noreferrer" class="text-green-600 !no-underline px-0.5"&gt;&lt;/a&gt;&lt;/span&gt;&lt;span&gt;â€‹.&lt;/span&gt;,rear_camera=&lt;span&gt;The POCO C65 is equipped with a 50MP AI triple camera setup, designed to capture high-quality photos with enhanced details and clarityâ€‹&lt;/span&gt;&lt;span class="" data-state="closed"&gt;&lt;a href="https://www.mi.com/uk/product/poco-c65/" target="_blank" rel="noopener noreferrer" class="text-green-600 !no-underline px-0.5"&gt;&lt;/a&gt;&lt;/span&gt;&lt;span&gt;â€‹.&lt;/span&gt;,front_camera=&lt;span data-key="spec_44" class="xm-text f-bold " data-type="text" data-id="4ad32f1282"&gt;Film Filter &lt;br /&gt;Â HDR mode&lt;br /&gt;Â Soft-light ring &lt;br /&gt;Â Portrait mode &lt;br /&gt;Â Time-lapse&lt;/span&gt;&lt;span data-key="spec_45" class="xm-text f-bold " data-type="text" data-id="985bdaa1cc"&gt;8MP front camera&lt;/span&gt;&lt;span data-key="spec_46" class="xm-text f-light " data-type="text" data-id="50239945c8"&gt;f/2.0&lt;/span&gt;,display=&lt;span&gt;The display on the POCO C65 is a 6.74" screen with a 90Hz refresh rate, designed for smooth scrolling and enhanced visual experience&lt;/span&gt;,battery_charging=&lt;span&gt;Â is equipped with a large 5000mAh battery, designed to support prolonged usage. It also supports 18W fast charging, enabling quick power-ups to keep you connected and productive throughout the day. This combination offers a balance between durability and convenience, making it suitable for extensive daily use.&lt;/span&gt;,cooling_system=The POCO C65's specific cooling system details are not mentioned in the available information. For cooling features or technologies used to manage heat during intensive operations,security_authentication=&lt;span&gt;For the POCO C65, security and authentication features typically include options like fingerprint sensors, face unlock, and possibly in-built software security measures to protect user data. These features ensure secure access to the device and safeguard personal information&lt;/span&gt;,nfc=supports multifunctional NFC, enabling convenient features like contactless payments, quick pairing with compatible devices, and easy data sharing.,network_connectivity=&lt;span&gt;The POCO C65 includes various network and connectivity options like 4G LTE, Wi-Fi, Bluetooth, and GPS. It also features multifunctional NFC for contactless transactions and device pairing&lt;/span&gt;,navigation=&lt;span&gt;The POCO C65 supports GPS, A-GPS, GLONASS, Beidou, and Galileo for comprehensive and accurate navigation capabilities, ensuring reliable location tracking across different regions and conditions&lt;/span&gt;,audio=&lt;span&gt;The POCO C65 features an audio system designed to deliver clear and immersive sound quality. It includes a 3.5mm headphone jack for compatibility with traditional wired headphones, ensuring users have flexibility in their choice of audio output.&lt;/span&gt;,sensor=&lt;strong&gt;&lt;span&gt;Virtual proximity sensor | Ambient light sensor | Accelerometer | Electronic compass&lt;/span&gt;&lt;/strong&gt;,operating_system=MIUI 14 for POCO*Availability of MIUI features, apps and services may vary depending on software version and phone model.,package_contents=Mobile Phone / Adapter / USB Type-C Cable / SIM Eject Tool / Quick Start Guide and Warranty Card / Safety Information*Contents in the package may differ across different regions.,rear_video_recording=&lt;span&gt;The POCO C65 supports front video recording, enhancing your video capturing capabilities.&lt;/span&gt;,video_playback=&lt;span&gt;The POCO C65 supports video playback, offering a great visual experience with its 6.74" HD+ display and 90Hz refresh rate.&lt;/span&gt;,data_transfer=&lt;span&gt;The POCO C65 offers data transfer features such as multifunctional NFC, a Type-C port for modern connectivity, and a 3.5mm headphone jack for traditional audio devices. These features facilitate versatile data sharing and connectivity options for users&lt;/span&gt;,dimensions=&lt;span data-key="spec_17" class="xm-text f-light " data-type="text" data-id="e30aa33e0b"&gt;Height: 168mm &lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_18" class="xm-text f-light " data-type="text" data-id="4324f2c478"&gt;Width: 78mm&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_19" class="xm-text f-light " data-type="text" data-id="c9750e593e"&gt;Thickness: 8.09mm&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_20" class="xm-text f-light " data-type="text" data-id="fdc5d72901"&gt;Weight: 192g&lt;/span&gt;&lt;span data-key="spec_21" class="xm-text f-light " data-type="text" data-id="bed668186a"&gt;*&lt;br /&gt;Data obtained from POCO laboratory. Industry measurement methods may vary, and therefore actual results may differ.&lt;/span&gt;,specifications=&lt;span&gt;The POCO C65 features a MediaTek Helio G85 processor, 6.74" 90Hz display, 50MP AI triple camera, 5000mAh battery, 18W fast charging, up to 16GB RAM with memory extension, 1TB storage expansion, side fingerprint sensor, and runs on MIUI 14 for POCOâ€‹&lt;/span&gt;&lt;span class="" data-state="closed"&gt;&lt;a href="https://www.mi.com/uk/product/poco-c65/" target="_blank" rel="noopener noreferrer" class="text-green-600 !no-underline px-0.5"&gt;&lt;/a&gt;&lt;/span&gt;&lt;span&gt;â€‹.&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>color=Black,ram=12GB,rom=512GB,processor=&lt;span data-key="spec_5" class="xm-text f-bold " data-type="text" data-id="effc52d893"&gt;Helio G99-Ultra&lt;/span&gt;&lt;span data-key="spec_6" class="xm-text f-light " data-type="text" data-id="0e3223a7ee"&gt;TSMC 6nm manufacturing process&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_7" class="xm-text f-light " data-type="text" data-id="308b50a033"&gt;CPUï¼š Octa-core processor 2 x Arm Cortex-A76, up to 2.2GHz 6 x Arm Cortex-A55, up to 2.0GHz&lt;/span&gt;&lt;span data-key="spec_8" class="xm-text f-light " data-type="text" data-id="a5c9ae0379"&gt;GPUï¼š ARM Mali-G57 MC2&lt;/span&gt;,rear_camera=&lt;span&gt;64MP+8MP+2MP triple camera&amp;nbsp;&lt;br&gt;&lt;span data-key="spec_46" class="xm-text f-bold " data-type="text" data-id="e800562df3"&gt;Rear camera photography features&lt;/span&gt;&lt;span data-key="spec_47" class="xm-text f-light " data-type="text" data-id="9c3b31007e"&gt;64MP mode | Night mode | Document mode | Film Camera | Portrait mode&lt;/span&gt;&lt;br&gt;&lt;/span&gt;,front_camera=&lt;span data-key="spec_57" class="xm-text f-bold " data-type="text" data-id="4ad32f1282"&gt;16MP front camera&lt;/span&gt;&lt;span data-key="spec_58" class="xm-text f-light " data-type="text" data-id="985bdaa1cc"&gt;f/2.45&amp;nbsp;&lt;br&gt;&lt;span data-key="spec_59" class="xm-text f-bold " data-type="text" data-id="2fdf4269c7"&gt;Front camera photography features &lt;br&gt;&lt;/span&gt;Night mode&lt;br&gt;Film Camera&lt;br&gt;Portrait mode&lt;br&gt;&lt;/span&gt;,display=&lt;span data-key="spec_22" class="xm-text f-bold " data-type="text" data-id="62023a1c0e"&gt;6.67" FHD+ Flow AMOLED DotDisplay&lt;/span&gt;&lt;span data-key="spec_23" class="xm-text f-light " data-type="text" data-id="6325f86c00"&gt;2400*1080, 394 ppi&lt;/span&gt;&lt;span data-key="spec_24" class="xm-text f-light " data-type="text" data-id="09007bdcc5"&gt;Contrast ratio: 5,000,000:1&lt;/span&gt;&lt;span data-key="spec_25" class="xm-text f-light " data-type="text" data-id="f031d76f85"&gt;Colour gamut: DCI-P3 wide colour gamut&lt;/span&gt;&lt;span data-key="spec_26" class="xm-text f-light " data-type="text" data-id="02324a2365"&gt;Brightness: 1000 nits (HBM), 1300 nits (peak)&lt;/span&gt;&lt;span data-key="spec_27" class="xm-text f-light " data-type="text" data-id="39feed82bf"&gt;Refresh rate: Up to 120Hz&lt;/span&gt;,battery_charging=&lt;span data-key="spec_70" class="xm-text f-light " data-type="text" data-id="4535c816f1"&gt;5000mAh (typ)&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_71" class="xm-text f-light " data-type="text" data-id="e2705627e0"&gt;67W wired turbo charging&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_72" class="xm-text f-light " data-type="text" data-id="264439ae59"&gt;67W in-box charger &lt;/span&gt;&lt;span data-key="spec_73" class="xm-text f-light " data-type="text" data-id="3b4b27fa9e"&gt;USB-C&lt;/span&gt;,cooling_system=The POCO M6 Pro features an advanced cooling system designed for optimal heat dissipation, ensuring smooth performance and preventing overheating during intensive use,security_authentication=&lt;span data-key="spec_75" class="xm-text f-light " data-type="text" data-id="0dc0744ecd"&gt;&lt;span&gt;The POCO M6 Pro includes security and authentication features to protect user data and ensure privacy&lt;/span&gt;&lt;br&gt;&lt;br&gt;In-screen fingerprint sensor&lt;br&gt;&lt;/span&gt;&lt;span data-key="spec_76" class="xm-text f-light " data-type="text" data-id="8cae001ad8"&gt;AI Face Unlock&lt;/span&gt;,nfc= enabling wireless communication between devices over short distances. This feature facilitates contactless payments, easy pairing with compatible devices, and quick data sharing.,network_connectivity=&lt;span&gt;&lt;br&gt;SIM1 + Hybrid* (SIM or MicroSD), supports dual 4G&lt;br&gt;&amp;nbsp;offers comprehensive network and connectivity options, ensuring users can stay connected in various environments and with multiple devices. It supports dual SIM functionality, allowing for versatile network usage.&lt;/span&gt;,navigation=&lt;span&gt;&lt;br&gt;GPS: L1 ï½œGLONASS: G1 | BDS: B1 | Galileo: E1&lt;br&gt;includes navigation features that utilize various satellite systems for accurate location tracking and mapping.&lt;/span&gt;,audio=&lt;span data-key="spec_95" class="xm-text f-light " data-type="text" data-id="544669ec9d"&gt;Dual speakers&lt;/span&gt;&lt;span data-key="spec_96" class="xm-text f-light " data-type="text" data-id="565928f0d8"&gt;3.5mm&amp;nbsp;&lt;br&gt;headphone jack&lt;br&gt;&lt;/span&gt;&lt;span data-key="spec_97" class="xm-text f-light " data-type="text" data-id="a78985a8a9"&gt;Dolby Atmos certification&lt;br&gt;&lt;/span&gt;&lt;span data-key="spec_98" class="xm-text f-light " data-type="text" data-id="5ba3fc8546"&gt;Hi-Res Audio certification&lt;br&gt;&lt;/span&gt;&lt;span data-key="spec_99" class="xm-text f-light " data-type="text" data-id="6ec848d980"&gt;Supports audio formats such as MP3 | FLAC | AAC | OGG | WAV&lt;/span&gt;,splash_water_dust_resistance=&lt;span data-key="spec_103" class="xm-text f-light " data-type="text" data-id="b39e83fc5b"&gt;IP54&lt;/span&gt;&lt;span data-key="spec_104" class="xm-text f-light " data-type="text" data-id="85040080f7"&gt;* &lt;br&gt;The device has been tested in a controlled environment and certified to be resistant to splash and dust in specific laboratory conditions with the classification IP54 under IEC 60529: 1989+A1:1999+A2:2013. Resistance is not permanent and may deteriorate naturally over time. If your device is wet, do not attempt to charge it. The life scene is different from the experimental environment. Do not immerse your smartphone in water completely or expose it to solutions such as seawater and chlorinated water or liquids such as drinks during daily use. Your warranty does not cover the damage caused by man-made immersion of your device in liquid. The test is conducted by TÃœV SÃœD Certification and Testing (China) Co., Ltd. Jiangsu Branch.&lt;/span&gt;,sensor=&lt;span&gt;The POCO M6 Pro is equipped with various sensors to enhance user experience and device functionality.&lt;br&gt;&lt;br&gt;Proximity sensor | Ambient light sensor | Accelerometer | Electronic compass | IR blaster ï½œGyroscope | Z-axis linear vibration motor&lt;/span&gt;,operating_system=MIUI 14 for POCO,rear_video_recording=&lt;span data-key="spec_52" class="xm-text f-bold " data-type="text" data-id="66c1cb5555"&gt;Rear camera video recording&lt;/span&gt;&lt;span data-key="spec_53" class="xm-text f-light " data-type="text" data-id="d36b6def57"&gt;1080p 1920Ã—1080 at 30fps/60fps&lt;/span&gt;&lt;span data-key="spec_54" class="xm-text f-light " data-type="text" data-id="314031b7bf"&gt;720p 1280Ã—720 at 30fps&lt;/span&gt;&lt;span data-key="spec_55" class="xm-text f-light " data-type="text" data-id="ff5535ab27"&gt;Slow motion video: 120fps, 720p&lt;/span&gt;,front_video_recording=&lt;span data-key="spec_66" class="xm-text f-bold " data-type="text" data-id="b07e125ed7"&gt;Front camera video recording&lt;/span&gt;&lt;span data-key="spec_67" class="xm-text f-light " data-type="text" data-id="4382a12439"&gt;1080p 1920Ã—1080 at 30fps/60fps&lt;/span&gt;&lt;span data-key="spec_68" class="xm-text f-light " data-type="text" data-id="c3aec946ef"&gt;720p 1280Ã—720 at 30fps&lt;/span&gt;,video_playback=&lt;span&gt;The POCO M6 Pro offers video playback capabilities designed to provide a high-quality viewing experience.&lt;/span&gt;,audio_playback=&lt;span&gt;The POCO M6 Pro is designed to provide an excellent audio playback experience.&lt;/span&gt;,data_transfer=&lt;span&gt;The POCO M6 Pro supports high-speed data transfer, ensuring swift and efficient file movement. This capability enhances user experience by reducing the time needed for data sharing between the device and other platforms or devices.&lt;/span&gt;,dimensions=&lt;span data-key="spec_16" class="xm-text f-light " data-type="text" data-id="e30aa33e0b"&gt;Height: 161.1mm&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_17" class="xm-text f-light " data-type="text" data-id="4324f2c478"&gt;Width: 74.95mm&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_18" class="xm-text f-light " data-type="text" data-id="c9750e593e"&gt;Thickness: 7.98mm&lt;br /&gt;&lt;/span&gt;&lt;span data-key="spec_19" class="xm-text f-light " data-type="text" data-id="fdc5d72901"&gt;Weight: 179g&lt;/span&gt;,specifications=&lt;span&gt;The POCO M6 Pro specs include a high-performance Helio G99 processor, ample storage and memory options, a large and vibrant AMOLED display, high-resolution cameras, and fast charging capabilities, alongside features like NFC, dual SIM support, and splash resistance, all powered by a user-friendly MIUI interface.&lt;/span&gt;</t>
   </si>
 </sst>
 </file>
@@ -499,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41BF6811-FA31-48AE-BD47-B83261575082}">
   <dimension ref="A1:A827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,8 +494,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -568,46 +539,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="1"/>
     </row>

</xml_diff>